<commit_message>
ADDED: Negative Test Cases
</commit_message>
<xml_diff>
--- a/build/resources/test/Bookswagon.xlsx
+++ b/build/resources/test/Bookswagon.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BooksWagon" sheetId="1" r:id="rId1"/>
+    <sheet name="invalid" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>email</t>
   </si>
@@ -88,6 +89,12 @@
   </si>
   <si>
     <t>The E Myth Revisited</t>
+  </si>
+  <si>
+    <t>Dinnu@248</t>
+  </si>
+  <si>
+    <t>dineshkumar.icon@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -424,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +532,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>22</v>
@@ -563,9 +570,110 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4" display="Dinnu@247"/>
+    <hyperlink ref="B3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2">
+        <v>515411</v>
+      </c>
+      <c r="L2">
+        <v>9542409637</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>